<commit_message>
correzione test-case RAD 11-12
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#01090800000000/AO Ordine Mauriziano/BABELE_WPF/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#01090800000000/AO Ordine Mauriziano/BABELE_WPF/1.0/report-checklist.xlsx
@@ -330,13 +330,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-04-07T12:07:46Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3c6f557188837555</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.10908.4.4.2.ebb5a850d128760d96b2b79d70970a7594bed1bdc05448067085db46238a465d.5848252548^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-04-26T14:54:54Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27f432ef90bf7684</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.10908.4.4.2.ebb5a850d128760d96b2b79d70970a7594bed1bdc05448067085db46238a465d.1962164a1d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">SI</t>
@@ -350,13 +350,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-04-07T12:11:54Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abe516ac296f4e25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.10908.4.4.2.ebb5a850d128760d96b2b79d70970a7594bed1bdc05448067085db46238a465d.daa4f07077^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2023-04-26T14:56:00Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">004f1f3dabc39e50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.10908.4.4.2.ebb5a850d128760d96b2b79d70970a7594bed1bdc05448067085db46238a465d.d0540f191a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RAD_CT3</t>
@@ -1593,7 +1593,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1670,18 +1670,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1822,7 +1810,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1968,74 +1956,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3381,17 +3301,17 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z1048576"/>
+  <dimension ref="A1:T1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P53" activeCellId="0" sqref="P53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="38.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="83.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="1" width="33.11"/>
@@ -3789,7 +3709,7 @@
         <v>60</v>
       </c>
       <c r="F14" s="28" t="n">
-        <v>45023</v>
+        <v>45042</v>
       </c>
       <c r="G14" s="29" t="s">
         <v>61</v>
@@ -3833,7 +3753,7 @@
         <v>66</v>
       </c>
       <c r="F15" s="28" t="n">
-        <v>45023</v>
+        <v>45042</v>
       </c>
       <c r="G15" s="29" t="s">
         <v>67</v>
@@ -4106,65 +4026,59 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" s="50" customFormat="true" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="37" t="n">
+    <row r="23" s="1" customFormat="true" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="25" t="n">
         <v>31</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="38" t="s">
+      <c r="D23" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="39" t="s">
+      <c r="E23" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="F23" s="40" t="n">
+      <c r="F23" s="28" t="n">
         <v>45030</v>
       </c>
-      <c r="G23" s="41" t="s">
+      <c r="G23" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="H23" s="42" t="s">
+      <c r="H23" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="I23" s="42" t="s">
+      <c r="I23" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="J23" s="43" t="s">
+      <c r="J23" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="K23" s="43"/>
-      <c r="L23" s="43" t="s">
+      <c r="K23" s="30"/>
+      <c r="L23" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="M23" s="43" t="s">
+      <c r="M23" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="N23" s="44" t="s">
+      <c r="N23" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="O23" s="43" t="s">
+      <c r="O23" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="P23" s="43" t="s">
+      <c r="P23" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="Q23" s="45"/>
-      <c r="R23" s="46"/>
-      <c r="S23" s="47"/>
-      <c r="T23" s="48" t="s">
+      <c r="Q23" s="34"/>
+      <c r="R23" s="31"/>
+      <c r="S23" s="32"/>
+      <c r="T23" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="U23" s="49"/>
-      <c r="V23" s="49"/>
-      <c r="W23" s="49"/>
-      <c r="X23" s="49"/>
-      <c r="Y23" s="49"/>
-      <c r="Z23" s="49"/>
     </row>
     <row r="24" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="25" t="n">
@@ -4268,65 +4182,59 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" s="50" customFormat="true" ht="135.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="37" t="n">
+    <row r="27" s="1" customFormat="true" ht="135.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="25" t="n">
         <v>39</v>
       </c>
-      <c r="B27" s="38" t="s">
+      <c r="B27" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="38" t="s">
+      <c r="C27" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="38" t="s">
+      <c r="D27" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="E27" s="39" t="s">
+      <c r="E27" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="F27" s="40" t="n">
+      <c r="F27" s="28" t="n">
         <v>45030</v>
       </c>
-      <c r="G27" s="51" t="s">
+      <c r="G27" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="H27" s="42" t="s">
+      <c r="H27" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="I27" s="42" t="s">
+      <c r="I27" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="J27" s="43" t="s">
+      <c r="J27" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="K27" s="43"/>
-      <c r="L27" s="43" t="s">
+      <c r="K27" s="30"/>
+      <c r="L27" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="M27" s="43" t="s">
+      <c r="M27" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="N27" s="44" t="s">
+      <c r="N27" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="O27" s="43" t="s">
+      <c r="O27" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="P27" s="43" t="s">
+      <c r="P27" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="Q27" s="52"/>
-      <c r="R27" s="46"/>
-      <c r="S27" s="47"/>
-      <c r="T27" s="48" t="s">
+      <c r="Q27" s="34"/>
+      <c r="R27" s="31"/>
+      <c r="S27" s="32"/>
+      <c r="T27" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="U27" s="49"/>
-      <c r="V27" s="49"/>
-      <c r="W27" s="49"/>
-      <c r="X27" s="49"/>
-      <c r="Y27" s="49"/>
-      <c r="Z27" s="49"/>
     </row>
     <row r="28" customFormat="false" ht="135.95" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="25" t="n">
@@ -4432,59 +4340,53 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" s="50" customFormat="true" ht="35.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="37" t="n">
+    <row r="31" s="1" customFormat="true" ht="35.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="25" t="n">
         <v>47</v>
       </c>
-      <c r="B31" s="38" t="s">
+      <c r="B31" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="38" t="s">
+      <c r="C31" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="38" t="s">
+      <c r="D31" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="E31" s="53" t="s">
+      <c r="E31" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="F31" s="40" t="n">
+      <c r="F31" s="28" t="n">
         <v>45030</v>
       </c>
-      <c r="G31" s="51" t="s">
+      <c r="G31" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="43" t="s">
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="K31" s="43"/>
-      <c r="L31" s="43" t="s">
+      <c r="K31" s="30"/>
+      <c r="L31" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="M31" s="43" t="s">
+      <c r="M31" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="N31" s="43"/>
-      <c r="O31" s="43"/>
-      <c r="P31" s="43" t="s">
+      <c r="N31" s="30"/>
+      <c r="O31" s="30"/>
+      <c r="P31" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="Q31" s="52"/>
-      <c r="R31" s="46" t="s">
+      <c r="Q31" s="34"/>
+      <c r="R31" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="S31" s="47"/>
-      <c r="T31" s="48" t="s">
+      <c r="S31" s="32"/>
+      <c r="T31" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="U31" s="49"/>
-      <c r="V31" s="49"/>
-      <c r="W31" s="49"/>
-      <c r="X31" s="49"/>
-      <c r="Y31" s="49"/>
-      <c r="Z31" s="49"/>
     </row>
     <row r="32" customFormat="false" ht="35.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="25" t="n">
@@ -4966,665 +4868,599 @@
         <v>88</v>
       </c>
     </row>
-    <row r="46" s="50" customFormat="true" ht="125.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="37" t="n">
+    <row r="46" s="1" customFormat="true" ht="125.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="25" t="n">
         <v>75</v>
       </c>
-      <c r="B46" s="38" t="s">
+      <c r="B46" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C46" s="38" t="s">
+      <c r="C46" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D46" s="38" t="s">
+      <c r="D46" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="E46" s="53" t="s">
+      <c r="E46" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="F46" s="40" t="n">
+      <c r="F46" s="28" t="n">
         <v>45033</v>
       </c>
-      <c r="G46" s="51" t="s">
+      <c r="G46" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="H46" s="42" t="s">
+      <c r="H46" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="I46" s="42" t="s">
+      <c r="I46" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="J46" s="43" t="s">
+      <c r="J46" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="K46" s="43"/>
-      <c r="L46" s="43" t="s">
+      <c r="K46" s="30"/>
+      <c r="L46" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="M46" s="43" t="s">
+      <c r="M46" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="N46" s="44" t="s">
+      <c r="N46" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="O46" s="43" t="s">
+      <c r="O46" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="P46" s="43" t="s">
+      <c r="P46" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="Q46" s="52"/>
-      <c r="R46" s="46"/>
-      <c r="S46" s="47"/>
-      <c r="T46" s="48" t="s">
+      <c r="Q46" s="34"/>
+      <c r="R46" s="31"/>
+      <c r="S46" s="32"/>
+      <c r="T46" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="U46" s="49"/>
-      <c r="V46" s="49"/>
-      <c r="W46" s="49"/>
-      <c r="X46" s="49"/>
-      <c r="Y46" s="49"/>
-      <c r="Z46" s="49"/>
-    </row>
-    <row r="47" s="50" customFormat="true" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="37" t="n">
+    </row>
+    <row r="47" s="1" customFormat="true" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="25" t="n">
         <v>76</v>
       </c>
-      <c r="B47" s="38" t="s">
+      <c r="B47" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C47" s="38" t="s">
+      <c r="C47" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D47" s="38" t="s">
+      <c r="D47" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="E47" s="53" t="s">
+      <c r="E47" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="F47" s="40" t="n">
+      <c r="F47" s="28" t="n">
         <v>45033</v>
       </c>
-      <c r="G47" s="42" t="s">
+      <c r="G47" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="H47" s="42" t="s">
+      <c r="H47" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="I47" s="42" t="s">
+      <c r="I47" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="J47" s="43" t="s">
+      <c r="J47" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="K47" s="43"/>
-      <c r="L47" s="43" t="s">
+      <c r="K47" s="30"/>
+      <c r="L47" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="M47" s="43" t="s">
+      <c r="M47" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="N47" s="44" t="s">
+      <c r="N47" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="O47" s="43" t="s">
+      <c r="O47" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="P47" s="43" t="s">
+      <c r="P47" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="Q47" s="43"/>
-      <c r="R47" s="46"/>
-      <c r="S47" s="47"/>
-      <c r="T47" s="48" t="s">
+      <c r="Q47" s="30"/>
+      <c r="R47" s="31"/>
+      <c r="S47" s="32"/>
+      <c r="T47" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="U47" s="49"/>
-      <c r="V47" s="49"/>
-      <c r="W47" s="49"/>
-      <c r="X47" s="49"/>
-      <c r="Y47" s="49"/>
-      <c r="Z47" s="49"/>
-    </row>
-    <row r="48" s="50" customFormat="true" ht="158.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="37" t="n">
+    </row>
+    <row r="48" s="1" customFormat="true" ht="158.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="25" t="n">
         <v>77</v>
       </c>
-      <c r="B48" s="38" t="s">
+      <c r="B48" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C48" s="38" t="s">
+      <c r="C48" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D48" s="38" t="s">
+      <c r="D48" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="E48" s="53" t="s">
+      <c r="E48" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="F48" s="40" t="n">
+      <c r="F48" s="28" t="n">
         <v>45033</v>
       </c>
-      <c r="G48" s="42" t="s">
+      <c r="G48" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="H48" s="42" t="s">
+      <c r="H48" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="I48" s="42" t="s">
+      <c r="I48" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="J48" s="43" t="s">
+      <c r="J48" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="K48" s="43"/>
-      <c r="L48" s="43" t="s">
+      <c r="K48" s="30"/>
+      <c r="L48" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="M48" s="43" t="s">
+      <c r="M48" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="N48" s="44" t="s">
+      <c r="N48" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="O48" s="43" t="s">
+      <c r="O48" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="P48" s="43" t="s">
+      <c r="P48" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="Q48" s="43"/>
-      <c r="R48" s="46"/>
-      <c r="S48" s="47"/>
-      <c r="T48" s="48" t="s">
+      <c r="Q48" s="30"/>
+      <c r="R48" s="31"/>
+      <c r="S48" s="32"/>
+      <c r="T48" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="U48" s="49"/>
-      <c r="V48" s="49"/>
-      <c r="W48" s="49"/>
-      <c r="X48" s="49"/>
-      <c r="Y48" s="49"/>
-      <c r="Z48" s="49"/>
-    </row>
-    <row r="49" s="50" customFormat="true" ht="135.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="37" t="n">
+    </row>
+    <row r="49" s="1" customFormat="true" ht="135.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="25" t="n">
         <v>78</v>
       </c>
-      <c r="B49" s="38" t="s">
+      <c r="B49" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C49" s="38" t="s">
+      <c r="C49" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D49" s="38" t="s">
+      <c r="D49" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="E49" s="53" t="s">
+      <c r="E49" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="F49" s="40" t="n">
+      <c r="F49" s="28" t="n">
         <v>45033</v>
       </c>
-      <c r="G49" s="42" t="s">
+      <c r="G49" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="H49" s="42" t="s">
+      <c r="H49" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="I49" s="42" t="s">
+      <c r="I49" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="J49" s="43" t="s">
+      <c r="J49" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="K49" s="43"/>
-      <c r="L49" s="43" t="s">
+      <c r="K49" s="30"/>
+      <c r="L49" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="M49" s="43" t="s">
+      <c r="M49" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="N49" s="44" t="s">
+      <c r="N49" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="O49" s="43" t="s">
+      <c r="O49" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="P49" s="43" t="s">
+      <c r="P49" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="Q49" s="43"/>
-      <c r="R49" s="46"/>
-      <c r="S49" s="47"/>
-      <c r="T49" s="48" t="s">
+      <c r="Q49" s="30"/>
+      <c r="R49" s="31"/>
+      <c r="S49" s="32"/>
+      <c r="T49" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="U49" s="49"/>
-      <c r="V49" s="49"/>
-      <c r="W49" s="49"/>
-      <c r="X49" s="49"/>
-      <c r="Y49" s="49"/>
-      <c r="Z49" s="49"/>
-    </row>
-    <row r="50" s="50" customFormat="true" ht="147.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="37" t="n">
+    </row>
+    <row r="50" s="1" customFormat="true" ht="147.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="25" t="n">
         <v>79</v>
       </c>
-      <c r="B50" s="38" t="s">
+      <c r="B50" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C50" s="38" t="s">
+      <c r="C50" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D50" s="38" t="s">
+      <c r="D50" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="E50" s="53" t="s">
+      <c r="E50" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="F50" s="40" t="n">
+      <c r="F50" s="28" t="n">
         <v>45033</v>
       </c>
-      <c r="G50" s="51" t="s">
+      <c r="G50" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="H50" s="42" t="s">
+      <c r="H50" s="29" t="s">
         <v>166</v>
       </c>
-      <c r="I50" s="42" t="s">
+      <c r="I50" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="J50" s="43" t="s">
+      <c r="J50" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="K50" s="43"/>
-      <c r="L50" s="43" t="s">
+      <c r="K50" s="30"/>
+      <c r="L50" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="M50" s="43" t="s">
+      <c r="M50" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="N50" s="44" t="s">
+      <c r="N50" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="O50" s="43" t="s">
+      <c r="O50" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="P50" s="43" t="s">
+      <c r="P50" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="Q50" s="43"/>
-      <c r="R50" s="46"/>
-      <c r="S50" s="47"/>
-      <c r="T50" s="48" t="s">
+      <c r="Q50" s="30"/>
+      <c r="R50" s="31"/>
+      <c r="S50" s="32"/>
+      <c r="T50" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="U50" s="49"/>
-      <c r="V50" s="49"/>
-      <c r="W50" s="49"/>
-      <c r="X50" s="49"/>
-      <c r="Y50" s="49"/>
-      <c r="Z50" s="49"/>
-    </row>
-    <row r="51" s="50" customFormat="true" ht="113.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="37" t="n">
+    </row>
+    <row r="51" s="1" customFormat="true" ht="113.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="25" t="n">
         <v>80</v>
       </c>
-      <c r="B51" s="38" t="s">
+      <c r="B51" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C51" s="38" t="s">
+      <c r="C51" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D51" s="38" t="s">
+      <c r="D51" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="E51" s="53" t="s">
+      <c r="E51" s="27" t="s">
         <v>170</v>
       </c>
-      <c r="F51" s="40" t="n">
+      <c r="F51" s="28" t="n">
         <v>45033</v>
       </c>
-      <c r="G51" s="51" t="s">
+      <c r="G51" s="29" t="s">
         <v>171</v>
       </c>
-      <c r="H51" s="42" t="s">
+      <c r="H51" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="I51" s="42" t="s">
+      <c r="I51" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="J51" s="43" t="s">
+      <c r="J51" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="K51" s="43"/>
-      <c r="L51" s="43" t="s">
+      <c r="K51" s="30"/>
+      <c r="L51" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="M51" s="43" t="s">
+      <c r="M51" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="N51" s="44" t="s">
+      <c r="N51" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="O51" s="43" t="s">
+      <c r="O51" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="P51" s="43" t="s">
+      <c r="P51" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="Q51" s="43"/>
-      <c r="R51" s="46"/>
-      <c r="S51" s="47"/>
-      <c r="T51" s="48" t="s">
+      <c r="Q51" s="30"/>
+      <c r="R51" s="31"/>
+      <c r="S51" s="32"/>
+      <c r="T51" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="U51" s="49"/>
-      <c r="V51" s="49"/>
-      <c r="W51" s="49"/>
-      <c r="X51" s="49"/>
-      <c r="Y51" s="49"/>
-      <c r="Z51" s="49"/>
-    </row>
-    <row r="52" s="50" customFormat="true" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="37" t="n">
+    </row>
+    <row r="52" s="1" customFormat="true" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="25" t="n">
         <v>81</v>
       </c>
-      <c r="B52" s="38" t="s">
+      <c r="B52" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C52" s="38" t="s">
+      <c r="C52" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D52" s="38" t="s">
+      <c r="D52" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="E52" s="53" t="s">
+      <c r="E52" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="F52" s="40" t="n">
+      <c r="F52" s="28" t="n">
         <v>45034</v>
       </c>
-      <c r="G52" s="42" t="s">
+      <c r="G52" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="H52" s="42" t="s">
+      <c r="H52" s="29" t="s">
         <v>178</v>
       </c>
-      <c r="I52" s="42" t="s">
+      <c r="I52" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="J52" s="43" t="s">
+      <c r="J52" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="K52" s="43"/>
-      <c r="L52" s="43" t="s">
+      <c r="K52" s="30"/>
+      <c r="L52" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="M52" s="43" t="s">
+      <c r="M52" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="N52" s="44" t="s">
+      <c r="N52" s="30" t="s">
         <v>180</v>
       </c>
-      <c r="O52" s="43" t="s">
+      <c r="O52" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="P52" s="43" t="s">
+      <c r="P52" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="Q52" s="43"/>
-      <c r="R52" s="46"/>
-      <c r="S52" s="47"/>
-      <c r="T52" s="48" t="s">
+      <c r="Q52" s="30"/>
+      <c r="R52" s="31"/>
+      <c r="S52" s="32"/>
+      <c r="T52" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="U52" s="49"/>
-      <c r="V52" s="49"/>
-      <c r="W52" s="49"/>
-      <c r="X52" s="49"/>
-      <c r="Y52" s="49"/>
-      <c r="Z52" s="49"/>
-    </row>
-    <row r="53" s="50" customFormat="true" ht="169.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="37" t="n">
+    </row>
+    <row r="53" s="1" customFormat="true" ht="169.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="25" t="n">
         <v>82</v>
       </c>
-      <c r="B53" s="38" t="s">
+      <c r="B53" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="38" t="s">
+      <c r="C53" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D53" s="38" t="s">
+      <c r="D53" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="E53" s="53" t="s">
+      <c r="E53" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="F53" s="40" t="n">
+      <c r="F53" s="28" t="n">
         <v>45034</v>
       </c>
-      <c r="G53" s="51" t="s">
+      <c r="G53" s="29" t="s">
         <v>183</v>
       </c>
-      <c r="H53" s="42" t="s">
+      <c r="H53" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="I53" s="42" t="s">
+      <c r="I53" s="29" t="s">
         <v>185</v>
       </c>
-      <c r="J53" s="43" t="s">
+      <c r="J53" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="K53" s="43"/>
-      <c r="L53" s="43" t="s">
+      <c r="K53" s="30"/>
+      <c r="L53" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="M53" s="43" t="s">
+      <c r="M53" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="N53" s="44" t="s">
+      <c r="N53" s="30" t="s">
         <v>186</v>
       </c>
-      <c r="O53" s="43" t="s">
+      <c r="O53" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="P53" s="43" t="s">
+      <c r="P53" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="Q53" s="43"/>
-      <c r="R53" s="46"/>
-      <c r="S53" s="47"/>
-      <c r="T53" s="48" t="s">
+      <c r="Q53" s="30"/>
+      <c r="R53" s="31"/>
+      <c r="S53" s="32"/>
+      <c r="T53" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="U53" s="49"/>
-      <c r="V53" s="49"/>
-      <c r="W53" s="49"/>
-      <c r="X53" s="49"/>
-      <c r="Y53" s="49"/>
-      <c r="Z53" s="49"/>
-    </row>
-    <row r="54" s="50" customFormat="true" ht="102.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="37" t="n">
+    </row>
+    <row r="54" s="1" customFormat="true" ht="102.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="25" t="n">
         <v>83</v>
       </c>
-      <c r="B54" s="38" t="s">
+      <c r="B54" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C54" s="38" t="s">
+      <c r="C54" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D54" s="38" t="s">
+      <c r="D54" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="E54" s="53" t="s">
+      <c r="E54" s="27" t="s">
         <v>188</v>
       </c>
-      <c r="F54" s="40" t="n">
+      <c r="F54" s="28" t="n">
         <v>45034</v>
       </c>
-      <c r="G54" s="51" t="s">
+      <c r="G54" s="29" t="s">
         <v>189</v>
       </c>
-      <c r="H54" s="42" t="s">
+      <c r="H54" s="29" t="s">
         <v>190</v>
       </c>
-      <c r="I54" s="42" t="s">
+      <c r="I54" s="29" t="s">
         <v>191</v>
       </c>
-      <c r="J54" s="43" t="s">
+      <c r="J54" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="K54" s="43"/>
-      <c r="L54" s="43" t="s">
+      <c r="K54" s="30"/>
+      <c r="L54" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="M54" s="43" t="s">
+      <c r="M54" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="N54" s="44" t="s">
+      <c r="N54" s="30" t="s">
         <v>192</v>
       </c>
-      <c r="O54" s="43" t="s">
+      <c r="O54" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="P54" s="43" t="s">
+      <c r="P54" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="Q54" s="43"/>
-      <c r="R54" s="46"/>
-      <c r="S54" s="47"/>
-      <c r="T54" s="48" t="s">
+      <c r="Q54" s="30"/>
+      <c r="R54" s="31"/>
+      <c r="S54" s="32"/>
+      <c r="T54" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="U54" s="49"/>
-      <c r="V54" s="49"/>
-      <c r="W54" s="49"/>
-      <c r="X54" s="49"/>
-      <c r="Y54" s="49"/>
-      <c r="Z54" s="49"/>
-    </row>
-    <row r="55" s="50" customFormat="true" ht="102.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="37" t="n">
+    </row>
+    <row r="55" s="1" customFormat="true" ht="102.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="25" t="n">
         <v>84</v>
       </c>
-      <c r="B55" s="38" t="s">
+      <c r="B55" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C55" s="38" t="s">
+      <c r="C55" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D55" s="38" t="s">
+      <c r="D55" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="E55" s="53" t="s">
+      <c r="E55" s="27" t="s">
         <v>194</v>
       </c>
-      <c r="F55" s="40" t="n">
+      <c r="F55" s="28" t="n">
         <v>45034</v>
       </c>
-      <c r="G55" s="51" t="s">
+      <c r="G55" s="29" t="s">
         <v>195</v>
       </c>
-      <c r="H55" s="42" t="s">
+      <c r="H55" s="29" t="s">
         <v>196</v>
       </c>
-      <c r="I55" s="42" t="s">
+      <c r="I55" s="29" t="s">
         <v>197</v>
       </c>
-      <c r="J55" s="43" t="s">
+      <c r="J55" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="K55" s="43"/>
-      <c r="L55" s="43" t="s">
+      <c r="K55" s="30"/>
+      <c r="L55" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="M55" s="43" t="s">
+      <c r="M55" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="N55" s="44" t="s">
+      <c r="N55" s="30" t="s">
         <v>198</v>
       </c>
-      <c r="O55" s="43" t="s">
+      <c r="O55" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="P55" s="43" t="s">
+      <c r="P55" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="Q55" s="43"/>
-      <c r="R55" s="46"/>
-      <c r="S55" s="47"/>
-      <c r="T55" s="48" t="s">
+      <c r="Q55" s="30"/>
+      <c r="R55" s="31"/>
+      <c r="S55" s="32"/>
+      <c r="T55" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="U55" s="49"/>
-      <c r="V55" s="49"/>
-      <c r="W55" s="49"/>
-      <c r="X55" s="49"/>
-      <c r="Y55" s="49"/>
-      <c r="Z55" s="49"/>
-    </row>
-    <row r="56" s="50" customFormat="true" ht="125.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="37" t="n">
+    </row>
+    <row r="56" s="1" customFormat="true" ht="125.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="25" t="n">
         <v>85</v>
       </c>
-      <c r="B56" s="38" t="s">
+      <c r="B56" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C56" s="38" t="s">
+      <c r="C56" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D56" s="38" t="s">
+      <c r="D56" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="E56" s="53" t="s">
+      <c r="E56" s="27" t="s">
         <v>200</v>
       </c>
-      <c r="F56" s="40" t="n">
+      <c r="F56" s="28" t="n">
         <v>45034</v>
       </c>
-      <c r="G56" s="51" t="s">
+      <c r="G56" s="29" t="s">
         <v>201</v>
       </c>
-      <c r="H56" s="42" t="s">
+      <c r="H56" s="29" t="s">
         <v>202</v>
       </c>
-      <c r="I56" s="42" t="s">
+      <c r="I56" s="29" t="s">
         <v>203</v>
       </c>
-      <c r="J56" s="43" t="s">
+      <c r="J56" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="K56" s="43"/>
-      <c r="L56" s="43" t="s">
+      <c r="K56" s="30"/>
+      <c r="L56" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="M56" s="43" t="s">
+      <c r="M56" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="N56" s="44" t="s">
+      <c r="N56" s="30" t="s">
         <v>204</v>
       </c>
-      <c r="O56" s="43" t="s">
+      <c r="O56" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="P56" s="43" t="s">
+      <c r="P56" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="Q56" s="43"/>
-      <c r="R56" s="46"/>
-      <c r="S56" s="47"/>
-      <c r="T56" s="48" t="s">
+      <c r="Q56" s="30"/>
+      <c r="R56" s="31"/>
+      <c r="S56" s="32"/>
+      <c r="T56" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="U56" s="49"/>
-      <c r="V56" s="49"/>
-      <c r="W56" s="49"/>
-      <c r="X56" s="49"/>
-      <c r="Y56" s="49"/>
-      <c r="Z56" s="49"/>
     </row>
     <row r="57" customFormat="false" ht="95.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="25" t="n">
@@ -17315,32 +17151,32 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="37" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="37" t="s">
         <v>322</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="37" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="37" t="s">
         <v>323</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="37" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="54"/>
-      <c r="B4" s="54"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -18398,10 +18234,10 @@
       <c r="B2" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="C2" s="55" t="s">
+      <c r="C2" s="38" t="s">
         <v>328</v>
       </c>
-      <c r="D2" s="55" t="s">
+      <c r="D2" s="38" t="s">
         <v>329</v>
       </c>
     </row>
@@ -18412,10 +18248,10 @@
       <c r="B3" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="38" t="s">
         <v>330</v>
       </c>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="38" t="s">
         <v>331</v>
       </c>
     </row>
@@ -18426,10 +18262,10 @@
       <c r="B4" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="38" t="s">
         <v>332</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="39" t="s">
         <v>333</v>
       </c>
     </row>
@@ -18440,10 +18276,10 @@
       <c r="B5" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="38" t="s">
         <v>335</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="38" t="s">
         <v>336</v>
       </c>
     </row>
@@ -18454,10 +18290,10 @@
       <c r="B6" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="38" t="s">
         <v>338</v>
       </c>
-      <c r="D6" s="56" t="s">
+      <c r="D6" s="39" t="s">
         <v>339</v>
       </c>
     </row>
@@ -18468,10 +18304,10 @@
       <c r="B7" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="38" t="s">
         <v>340</v>
       </c>
-      <c r="D7" s="56" t="s">
+      <c r="D7" s="39" t="s">
         <v>341</v>
       </c>
     </row>
@@ -18482,10 +18318,10 @@
       <c r="B8" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="38" t="s">
         <v>342</v>
       </c>
-      <c r="D8" s="56" t="s">
+      <c r="D8" s="39" t="s">
         <v>343</v>
       </c>
     </row>
@@ -18496,10 +18332,10 @@
       <c r="B9" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="38" t="s">
         <v>345</v>
       </c>
-      <c r="D9" s="56" t="s">
+      <c r="D9" s="39" t="s">
         <v>346</v>
       </c>
     </row>
@@ -18510,10 +18346,10 @@
       <c r="B10" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="C10" s="55" t="n">
+      <c r="C10" s="38" t="n">
         <v>191</v>
       </c>
-      <c r="D10" s="55" t="s">
+      <c r="D10" s="38" t="s">
         <v>348</v>
       </c>
     </row>
@@ -18524,10 +18360,10 @@
       <c r="B11" s="11" t="s">
         <v>349</v>
       </c>
-      <c r="C11" s="55" t="n">
+      <c r="C11" s="38" t="n">
         <v>192</v>
       </c>
-      <c r="D11" s="55" t="s">
+      <c r="D11" s="38" t="s">
         <v>350</v>
       </c>
     </row>
@@ -18538,10 +18374,10 @@
       <c r="B12" s="11" t="s">
         <v>349</v>
       </c>
-      <c r="C12" s="55" t="n">
+      <c r="C12" s="38" t="n">
         <v>208</v>
       </c>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="38" t="s">
         <v>351</v>
       </c>
     </row>
@@ -18552,10 +18388,10 @@
       <c r="B13" s="11" t="s">
         <v>349</v>
       </c>
-      <c r="C13" s="55" t="n">
+      <c r="C13" s="38" t="n">
         <v>224</v>
       </c>
-      <c r="D13" s="56" t="s">
+      <c r="D13" s="39" t="s">
         <v>352</v>
       </c>
     </row>
@@ -18566,10 +18402,10 @@
       <c r="B14" s="11" t="s">
         <v>349</v>
       </c>
-      <c r="C14" s="55" t="n">
+      <c r="C14" s="38" t="n">
         <v>240</v>
       </c>
-      <c r="D14" s="55" t="s">
+      <c r="D14" s="38" t="s">
         <v>353</v>
       </c>
     </row>
@@ -18580,10 +18416,10 @@
       <c r="B15" s="11" t="s">
         <v>349</v>
       </c>
-      <c r="C15" s="55" t="n">
+      <c r="C15" s="38" t="n">
         <v>256</v>
       </c>
-      <c r="D15" s="56" t="s">
+      <c r="D15" s="39" t="s">
         <v>354</v>
       </c>
     </row>
@@ -18594,10 +18430,10 @@
       <c r="B16" s="11" t="s">
         <v>349</v>
       </c>
-      <c r="C16" s="55" t="n">
+      <c r="C16" s="38" t="n">
         <v>272</v>
       </c>
-      <c r="D16" s="56" t="s">
+      <c r="D16" s="39" t="s">
         <v>355</v>
       </c>
     </row>
@@ -18608,10 +18444,10 @@
       <c r="B17" s="11" t="s">
         <v>349</v>
       </c>
-      <c r="C17" s="55" t="n">
+      <c r="C17" s="38" t="n">
         <v>288</v>
       </c>
-      <c r="D17" s="56" t="s">
+      <c r="D17" s="39" t="s">
         <v>356</v>
       </c>
     </row>
@@ -18622,10 +18458,10 @@
       <c r="B18" s="11" t="s">
         <v>349</v>
       </c>
-      <c r="C18" s="55" t="n">
+      <c r="C18" s="38" t="n">
         <v>304</v>
       </c>
-      <c r="D18" s="56" t="s">
+      <c r="D18" s="39" t="s">
         <v>357</v>
       </c>
     </row>
@@ -18636,10 +18472,10 @@
       <c r="B19" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="C19" s="55" t="n">
+      <c r="C19" s="38" t="n">
         <v>193</v>
       </c>
-      <c r="D19" s="55" t="s">
+      <c r="D19" s="38" t="s">
         <v>359</v>
       </c>
     </row>
@@ -18650,10 +18486,10 @@
       <c r="B20" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="C20" s="55" t="n">
+      <c r="C20" s="38" t="n">
         <v>209</v>
       </c>
-      <c r="D20" s="55" t="s">
+      <c r="D20" s="38" t="s">
         <v>360</v>
       </c>
     </row>
@@ -18664,10 +18500,10 @@
       <c r="B21" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="C21" s="55" t="n">
+      <c r="C21" s="38" t="n">
         <v>225</v>
       </c>
-      <c r="D21" s="56" t="s">
+      <c r="D21" s="39" t="s">
         <v>361</v>
       </c>
     </row>
@@ -18678,10 +18514,10 @@
       <c r="B22" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="C22" s="55" t="n">
+      <c r="C22" s="38" t="n">
         <v>241</v>
       </c>
-      <c r="D22" s="55" t="s">
+      <c r="D22" s="38" t="s">
         <v>362</v>
       </c>
     </row>
@@ -18692,10 +18528,10 @@
       <c r="B23" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="C23" s="55" t="n">
+      <c r="C23" s="38" t="n">
         <v>257</v>
       </c>
-      <c r="D23" s="56" t="s">
+      <c r="D23" s="39" t="s">
         <v>363</v>
       </c>
     </row>
@@ -18706,10 +18542,10 @@
       <c r="B24" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="C24" s="55" t="n">
+      <c r="C24" s="38" t="n">
         <v>273</v>
       </c>
-      <c r="D24" s="56" t="s">
+      <c r="D24" s="39" t="s">
         <v>364</v>
       </c>
     </row>
@@ -18720,10 +18556,10 @@
       <c r="B25" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="C25" s="55" t="n">
+      <c r="C25" s="38" t="n">
         <v>289</v>
       </c>
-      <c r="D25" s="56" t="s">
+      <c r="D25" s="39" t="s">
         <v>365</v>
       </c>
     </row>
@@ -18734,10 +18570,10 @@
       <c r="B26" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="C26" s="55" t="n">
+      <c r="C26" s="38" t="n">
         <v>305</v>
       </c>
-      <c r="D26" s="56" t="s">
+      <c r="D26" s="39" t="s">
         <v>366</v>
       </c>
     </row>
@@ -18748,10 +18584,10 @@
       <c r="B27" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="C27" s="55" t="n">
+      <c r="C27" s="38" t="n">
         <v>194</v>
       </c>
-      <c r="D27" s="55" t="s">
+      <c r="D27" s="38" t="s">
         <v>368</v>
       </c>
     </row>
@@ -18762,10 +18598,10 @@
       <c r="B28" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="C28" s="55" t="n">
+      <c r="C28" s="38" t="n">
         <v>210</v>
       </c>
-      <c r="D28" s="55" t="s">
+      <c r="D28" s="38" t="s">
         <v>369</v>
       </c>
     </row>
@@ -18776,10 +18612,10 @@
       <c r="B29" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="C29" s="55" t="n">
+      <c r="C29" s="38" t="n">
         <v>226</v>
       </c>
-      <c r="D29" s="57" t="s">
+      <c r="D29" s="40" t="s">
         <v>370</v>
       </c>
     </row>
@@ -18790,10 +18626,10 @@
       <c r="B30" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="C30" s="55" t="n">
+      <c r="C30" s="38" t="n">
         <v>242</v>
       </c>
-      <c r="D30" s="55" t="s">
+      <c r="D30" s="38" t="s">
         <v>371</v>
       </c>
     </row>
@@ -18804,10 +18640,10 @@
       <c r="B31" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="C31" s="55" t="n">
+      <c r="C31" s="38" t="n">
         <v>258</v>
       </c>
-      <c r="D31" s="56" t="s">
+      <c r="D31" s="39" t="s">
         <v>372</v>
       </c>
     </row>
@@ -18818,10 +18654,10 @@
       <c r="B32" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="C32" s="55" t="n">
+      <c r="C32" s="38" t="n">
         <v>274</v>
       </c>
-      <c r="D32" s="56" t="s">
+      <c r="D32" s="39" t="s">
         <v>373</v>
       </c>
     </row>
@@ -18832,10 +18668,10 @@
       <c r="B33" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="C33" s="55" t="n">
+      <c r="C33" s="38" t="n">
         <v>290</v>
       </c>
-      <c r="D33" s="56" t="s">
+      <c r="D33" s="39" t="s">
         <v>374</v>
       </c>
     </row>
@@ -18846,10 +18682,10 @@
       <c r="B34" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="C34" s="55" t="n">
+      <c r="C34" s="38" t="n">
         <v>306</v>
       </c>
-      <c r="D34" s="56" t="s">
+      <c r="D34" s="39" t="s">
         <v>375</v>
       </c>
     </row>
@@ -18860,10 +18696,10 @@
       <c r="B35" s="11" t="s">
         <v>376</v>
       </c>
-      <c r="C35" s="55" t="n">
+      <c r="C35" s="38" t="n">
         <v>195</v>
       </c>
-      <c r="D35" s="55" t="n">
+      <c r="D35" s="38" t="n">
         <v>204</v>
       </c>
     </row>
@@ -18874,10 +18710,10 @@
       <c r="B36" s="11" t="s">
         <v>376</v>
       </c>
-      <c r="C36" s="55" t="n">
+      <c r="C36" s="38" t="n">
         <v>211</v>
       </c>
-      <c r="D36" s="55" t="n">
+      <c r="D36" s="38" t="n">
         <v>220</v>
       </c>
     </row>
@@ -18888,10 +18724,10 @@
       <c r="B37" s="11" t="s">
         <v>376</v>
       </c>
-      <c r="C37" s="55" t="n">
+      <c r="C37" s="38" t="n">
         <v>227</v>
       </c>
-      <c r="D37" s="56" t="n">
+      <c r="D37" s="39" t="n">
         <v>236</v>
       </c>
     </row>
@@ -18902,10 +18738,10 @@
       <c r="B38" s="11" t="s">
         <v>376</v>
       </c>
-      <c r="C38" s="55" t="n">
+      <c r="C38" s="38" t="n">
         <v>243</v>
       </c>
-      <c r="D38" s="55" t="n">
+      <c r="D38" s="38" t="n">
         <v>252</v>
       </c>
     </row>
@@ -18916,10 +18752,10 @@
       <c r="B39" s="11" t="s">
         <v>376</v>
       </c>
-      <c r="C39" s="55" t="n">
+      <c r="C39" s="38" t="n">
         <v>259</v>
       </c>
-      <c r="D39" s="56" t="n">
+      <c r="D39" s="39" t="n">
         <v>268</v>
       </c>
     </row>
@@ -18930,10 +18766,10 @@
       <c r="B40" s="11" t="s">
         <v>376</v>
       </c>
-      <c r="C40" s="55" t="n">
+      <c r="C40" s="38" t="n">
         <v>275</v>
       </c>
-      <c r="D40" s="56" t="n">
+      <c r="D40" s="39" t="n">
         <v>284</v>
       </c>
     </row>
@@ -18944,10 +18780,10 @@
       <c r="B41" s="11" t="s">
         <v>376</v>
       </c>
-      <c r="C41" s="55" t="n">
+      <c r="C41" s="38" t="n">
         <v>291</v>
       </c>
-      <c r="D41" s="56" t="n">
+      <c r="D41" s="39" t="n">
         <v>300</v>
       </c>
     </row>
@@ -18958,10 +18794,10 @@
       <c r="B42" s="11" t="s">
         <v>376</v>
       </c>
-      <c r="C42" s="55" t="n">
+      <c r="C42" s="38" t="n">
         <v>307</v>
       </c>
-      <c r="D42" s="56" t="n">
+      <c r="D42" s="39" t="n">
         <v>316</v>
       </c>
     </row>
@@ -18972,10 +18808,10 @@
       <c r="B43" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="C43" s="55" t="n">
+      <c r="C43" s="38" t="n">
         <v>196</v>
       </c>
-      <c r="D43" s="55" t="n">
+      <c r="D43" s="38" t="n">
         <v>207</v>
       </c>
     </row>
@@ -18986,10 +18822,10 @@
       <c r="B44" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="C44" s="55" t="n">
+      <c r="C44" s="38" t="n">
         <v>212</v>
       </c>
-      <c r="D44" s="55" t="n">
+      <c r="D44" s="38" t="n">
         <v>223</v>
       </c>
     </row>
@@ -19000,10 +18836,10 @@
       <c r="B45" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="C45" s="55" t="n">
+      <c r="C45" s="38" t="n">
         <v>228</v>
       </c>
-      <c r="D45" s="56" t="n">
+      <c r="D45" s="39" t="n">
         <v>239</v>
       </c>
     </row>
@@ -19014,10 +18850,10 @@
       <c r="B46" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="C46" s="55" t="n">
+      <c r="C46" s="38" t="n">
         <v>244</v>
       </c>
-      <c r="D46" s="55" t="n">
+      <c r="D46" s="38" t="n">
         <v>255</v>
       </c>
     </row>
@@ -19028,10 +18864,10 @@
       <c r="B47" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="C47" s="55" t="n">
+      <c r="C47" s="38" t="n">
         <v>260</v>
       </c>
-      <c r="D47" s="56" t="n">
+      <c r="D47" s="39" t="n">
         <v>271</v>
       </c>
     </row>
@@ -19042,10 +18878,10 @@
       <c r="B48" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="C48" s="55" t="n">
+      <c r="C48" s="38" t="n">
         <v>276</v>
       </c>
-      <c r="D48" s="56" t="n">
+      <c r="D48" s="39" t="n">
         <v>287</v>
       </c>
     </row>
@@ -19056,10 +18892,10 @@
       <c r="B49" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="C49" s="55" t="n">
+      <c r="C49" s="38" t="n">
         <v>292</v>
       </c>
-      <c r="D49" s="56" t="n">
+      <c r="D49" s="39" t="n">
         <v>303</v>
       </c>
     </row>
@@ -19070,10 +18906,10 @@
       <c r="B50" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="C50" s="55" t="n">
+      <c r="C50" s="38" t="n">
         <v>308</v>
       </c>
-      <c r="D50" s="56" t="n">
+      <c r="D50" s="39" t="n">
         <v>319</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correzione report-checklist colonne: F, G, H, I, L, M, O, P
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#01090800000000/AO Ordine Mauriziano/BABELE_WPF/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#01090800000000/AO Ordine Mauriziano/BABELE_WPF/1.0/report-checklist.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="577">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -2767,7 +2767,7 @@
   <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="O96 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3841,7 +3841,7 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="O96 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4950,11 +4950,11 @@
   <dimension ref="A1:T1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="I90" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="K89" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A90" activeCellId="0" sqref="A90"/>
-      <selection pane="bottomRight" activeCell="Q96" activeCellId="0" sqref="Q96"/>
+      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="A89" activeCellId="0" sqref="A89"/>
+      <selection pane="bottomRight" activeCell="O96" activeCellId="0" sqref="O96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6369,7 +6369,9 @@
       <c r="N34" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="O34" s="30"/>
+      <c r="O34" s="30" t="s">
+        <v>58</v>
+      </c>
       <c r="P34" s="30" t="s">
         <v>142</v>
       </c>
@@ -6475,7 +6477,9 @@
       <c r="N36" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="O36" s="30"/>
+      <c r="O36" s="30" t="s">
+        <v>58</v>
+      </c>
       <c r="P36" s="30" t="s">
         <v>155</v>
       </c>
@@ -9243,7 +9247,9 @@
       <c r="N94" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="O94" s="30"/>
+      <c r="O94" s="30" t="s">
+        <v>58</v>
+      </c>
       <c r="P94" s="30" t="s">
         <v>142</v>
       </c>
@@ -9349,7 +9355,9 @@
       <c r="N96" s="30" t="s">
         <v>434</v>
       </c>
-      <c r="O96" s="30"/>
+      <c r="O96" s="30" t="s">
+        <v>58</v>
+      </c>
       <c r="P96" s="30" t="s">
         <v>155</v>
       </c>
@@ -15153,8 +15161,8 @@
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A6:B6"/>
   </mergeCells>
-  <dataValidations count="7">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J10 L10:M13 O10:O13 J22 J26 J30 J34:J41 L42:M43 O42:O43 J44 L45:M45 O45 L90:M93 O90:O93 J91:J111 L100:M101 O100:O101 L107:M111 O107:O111 J113 L113:M116 O113:O116" type="list">
+  <dataValidations count="9">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J10 L10:M13 O10:O13 J22 J26 J30 J34:J41 L42:M43 J44 L45:M45 L90:M93 J91:J95 J97:J111 L100:M101 L107:M111 J113 L113:M116" type="list">
       <formula1>Sheet1!$B$2:$B$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -15162,7 +15170,7 @@
       <formula1>Sheet1!$A$2:$A$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J14:J17 L14:M41 O14:O41 L44:M44 O44 L46:M89 O46:O89 L94:M99 O94:O99 L102:M106 O102:O106 L112:M112 O112" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J14:J17 L14:M41 L44:M44 L46:M89 L94:M99 L102:M106 L112:M112" type="list">
       <formula1>Summary!$B$2:$B$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -15180,6 +15188,14 @@
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J11:J13 J18:J21 J25 J29 J33 J42:J43 J45 J65:J89 J114:J115" type="list">
       <formula1>Summary!$B$2:$B$3</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J96" type="list">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O14:O116" type="list">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -15205,7 +15221,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="1" sqref="O96 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16886,7 +16902,7 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="O96 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>